<commit_message>
Output content of Excel file to README.md
</commit_message>
<xml_diff>
--- a/Internship_list.xlsx
+++ b/Internship_list.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jimkellypercine/Desktop/Brandeis_internship/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jimkellypercine/Desktop/Brandeis_internship_search/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54E246F3-D03E-AA49-AB57-7CE0E2492BBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D69B4E7-7418-7B4F-AFC4-A6012C788B21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16940" xr2:uid="{E5EF8726-1FCE-1B45-A9E5-5959CF12D92D}"/>
+    <workbookView xWindow="60" yWindow="500" windowWidth="28040" windowHeight="16940" xr2:uid="{E5EF8726-1FCE-1B45-A9E5-5959CF12D92D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="10">
   <si>
     <t>FaceBook</t>
   </si>
@@ -53,23 +53,37 @@
     <t>Publicis Sapient</t>
   </si>
   <si>
-    <t>COMPANIES</t>
-  </si>
-  <si>
-    <t>LINKS</t>
-  </si>
-  <si>
     <t>NOTES</t>
+  </si>
+  <si>
+    <t>COMPANY</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Great Time</t>
+  </si>
+  <si>
+    <t>jpe@gmail.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -92,13 +106,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -414,48 +431,86 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" t="s">
         <v>5</v>
-      </c>
-      <c r="B1" t="s">
-        <v>6</v>
       </c>
       <c r="C1" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+      <c r="A2" s="1" t="s">
         <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>1</v>
       </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>3</v>
       </c>
+      <c r="B5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>4</v>
       </c>
+      <c r="B6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>9</v>
+      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" location="fpstate=tldetail&amp;htivrt=jobs&amp;htiq=facebook+internship&amp;htidocid=kBV7bWXmAS4AAAAAAAAAAA%3D%3D" xr:uid="{909DAFEB-92DE-BB49-A30E-93C06EEED98B}"/>
+    <hyperlink ref="C2" r:id="rId2" xr:uid="{8618966E-5F5F-0E4B-88B5-065B316B3433}"/>
+    <hyperlink ref="C3" r:id="rId3" xr:uid="{C446EC75-242A-584F-A922-3FB884B0CC6B}"/>
+    <hyperlink ref="C4" r:id="rId4" xr:uid="{2C085D38-CBEB-D640-8234-C83D3873C5EE}"/>
+    <hyperlink ref="C5" r:id="rId5" xr:uid="{80CF4788-BA5C-E44C-9909-87342E820839}"/>
+    <hyperlink ref="C6" r:id="rId6" xr:uid="{03533F32-37A0-914D-8409-D169F14CD492}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
update with new column
</commit_message>
<xml_diff>
--- a/Internship_list.xlsx
+++ b/Internship_list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jimkellypercine/Desktop/Brandeis_internship_search/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A25D6E04-CDDE-264A-9C79-4712CD1B29A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E116BE4-4D3E-B24A-B887-046D26FCDFBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3820" yWindow="1020" windowWidth="28040" windowHeight="16940" xr2:uid="{E5EF8726-1FCE-1B45-A9E5-5959CF12D92D}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="46">
   <si>
     <t>Amazon</t>
   </si>
@@ -53,9 +53,6 @@
     <t>COMPANY</t>
   </si>
   <si>
-    <t>EMAIL</t>
-  </si>
-  <si>
     <t>RANK 1-5</t>
   </si>
   <si>
@@ -68,27 +65,15 @@
     <t>Start practicing behavioral/basic interview questions (questions about what you would do in certain situations in the workspace) and have in your mind certain experiences from your life that you can draw from to answer them.</t>
   </si>
   <si>
-    <t>fduverglas@brandeis.edu</t>
-  </si>
-  <si>
     <t>PayPal</t>
   </si>
   <si>
     <t>Prepare early, apply early, don’t be discouraged</t>
   </si>
   <si>
-    <t>danielhariyanto@brandeis.edu</t>
-  </si>
-  <si>
-    <t>blacy@brandeis.edu</t>
-  </si>
-  <si>
     <t>When you take the time outside the classroom to develop your skills in practical area in which you enjoy your employer will take notice and it will benefit you in the long run in comparison to those who don't take the initiative to hold themselves accountable while they pursue things in which they are most passionate.</t>
   </si>
   <si>
-    <t>andrewng@brandeis.edu</t>
-  </si>
-  <si>
     <t>CommScope</t>
   </si>
   <si>
@@ -98,75 +83,51 @@
     <t xml:space="preserve">1. start apply early (I started applying around June and got the first offer late August for next year internship) 2. build a great resume (ask your friends, people in the industry to read your resume, the more the better), do side projects, hackathons, etc... things that showcase the skills that companies are looking for </t>
   </si>
   <si>
-    <t>rick@treitman.com</t>
-  </si>
-  <si>
     <t>Get started early.</t>
   </si>
   <si>
     <t>Adobe</t>
   </si>
   <si>
-    <t>steve.beckhardt@gmail.com</t>
-  </si>
-  <si>
     <t>Sonos</t>
   </si>
   <si>
     <t>Gnar company</t>
   </si>
   <si>
-    <t>lfreed@irobot.com</t>
-  </si>
-  <si>
     <t>iRobot</t>
   </si>
   <si>
     <t>Talk about yourself. projects, things you did to apply that knowledge you have from school</t>
   </si>
   <si>
-    <t>rstachel@gmail.com</t>
-  </si>
-  <si>
     <t>I'm retired so I don't have direct contacts. But looking outside the computer industry in technology driven areas like health care might be promising. Biotech, in Massachusetts. Emphasize data science skills.</t>
   </si>
   <si>
     <t>Bob Stachel</t>
   </si>
   <si>
-    <t>jameskong@brandeis.edu</t>
-  </si>
-  <si>
     <t>Zebra Technologies</t>
   </si>
   <si>
+    <t>https://www.zebra.com/us/en/about-zebra/careers.html</t>
+  </si>
+  <si>
     <t>apply to a BUNCH, no such thing as too many as you can apply to 100 and still not get an interview, don't lose hope, also make sure to get your leetcode practice in</t>
   </si>
   <si>
-    <t>nicholas.gordon@shopify.com</t>
-  </si>
-  <si>
     <t>Shopify</t>
   </si>
   <si>
     <t>find a connection, be it someone you actually know (or can be introduced to) or generate ("hey we have X in common and I'm looking at your company", for example "we both went to Brandeis")</t>
   </si>
   <si>
-    <t>jered@convivian.com</t>
-  </si>
-  <si>
     <t>Red Hat</t>
   </si>
   <si>
     <t>Have past experience or an interest in open source software</t>
   </si>
   <si>
-    <t>shuranli@brandeis.edu</t>
-  </si>
-  <si>
-    <t>clarajnice@gmail.com</t>
-  </si>
-  <si>
     <t>Squarespace</t>
   </si>
   <si>
@@ -179,7 +140,40 @@
     <t xml:space="preserve">LEARN Academy is trying to promote internships in the Ruby/Rails community. </t>
   </si>
   <si>
-    <t>chantelle@learnacademy.org</t>
+    <t>https://www.publicissapient.com/</t>
+  </si>
+  <si>
+    <t>http://paypal.com/</t>
+  </si>
+  <si>
+    <t>http://microsoft.com/</t>
+  </si>
+  <si>
+    <t>https://jobs.commscope.com/search/?createNewAlert=false&amp;q=&amp;locationsearch=&amp;optionsFacetsDD_title=&amp;optionsFacetsDD_department=Early+Careers&amp;optionsFacetsDD_location=&amp;optionsFacetsDD_country=</t>
+  </si>
+  <si>
+    <t>https://careers.imc.com/ap/en/c/internships-jobs</t>
+  </si>
+  <si>
+    <t>https://irobot.wd5.myworkdayjobs.com/iRobot?_ga=2.144828087.2021781397.1627654807-1547478520.1627654805</t>
+  </si>
+  <si>
+    <t>https://careers-redhat.icims.com/jobs/search?ss=1&amp;searchKeyword=internship</t>
+  </si>
+  <si>
+    <t>https://www.squarespace.com/careers/early-career</t>
+  </si>
+  <si>
+    <t>https://careers.google.com/jobs/results/?employment_type=INTERN&amp;jlo=en_US&amp;q=STEP</t>
+  </si>
+  <si>
+    <t>Application List</t>
+  </si>
+  <si>
+    <t>/</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> https://www.shopify.com/careers/dev-degree-2023-remote-americas_8f2a8000-42e4-49a9-b0ec-d84bc367bb0f</t>
   </si>
 </sst>
 </file>
@@ -556,7 +550,7 @@
   <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:D17"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -564,7 +558,7 @@
     <col min="1" max="1" width="10.83203125" style="1"/>
     <col min="2" max="2" width="10.83203125" style="1" customWidth="1"/>
     <col min="3" max="3" width="20.33203125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="10.83203125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="16.83203125" style="1" customWidth="1"/>
     <col min="5" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
@@ -573,27 +567,27 @@
         <v>4</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>5</v>
+        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="102" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="1">
+        <v>5</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="1">
-        <v>5</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>41</v>
+      <c r="D2" s="2" t="s">
+        <v>42</v>
       </c>
       <c r="E2" s="3"/>
     </row>
@@ -605,25 +599,25 @@
         <v>5</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>10</v>
+        <v>34</v>
       </c>
       <c r="E3" s="4"/>
     </row>
     <row r="4" spans="1:5" ht="51" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B4" s="1">
         <v>5</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>13</v>
+        <v>35</v>
       </c>
       <c r="E4" s="3"/>
     </row>
@@ -635,10 +629,10 @@
         <v>5</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>13</v>
+        <v>36</v>
       </c>
       <c r="E5" s="3"/>
     </row>
@@ -650,171 +644,171 @@
         <v>5</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>14</v>
+        <v>36</v>
       </c>
       <c r="E6" s="3"/>
     </row>
     <row r="7" spans="1:5" ht="272" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="B7" s="1">
         <v>5</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>16</v>
+        <v>37</v>
       </c>
       <c r="E7" s="3"/>
     </row>
     <row r="8" spans="1:5" ht="204" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="B8" s="1">
         <v>5</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>45</v>
+        <v>32</v>
       </c>
       <c r="D8" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E8" s="3"/>
+    </row>
+    <row r="9" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E8" s="3"/>
-    </row>
-    <row r="9" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="A9" s="1" t="s">
-        <v>22</v>
-      </c>
       <c r="B9" s="1">
         <v>5</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>20</v>
+        <v>44</v>
       </c>
       <c r="E9" s="3"/>
     </row>
-    <row r="10" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="B10" s="1">
         <v>5</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>23</v>
+        <v>44</v>
       </c>
       <c r="E10" s="3"/>
     </row>
     <row r="11" spans="1:5" ht="68" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="B11" s="1">
         <v>5</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>46</v>
+        <v>33</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="E11" s="3"/>
     </row>
     <row r="12" spans="1:5" ht="85" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="B12" s="1">
         <v>5</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>26</v>
+        <v>39</v>
       </c>
       <c r="E12" s="3"/>
     </row>
     <row r="13" spans="1:5" ht="187" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="B13" s="1">
         <v>5</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>29</v>
+        <v>44</v>
       </c>
       <c r="E13" s="3"/>
     </row>
     <row r="14" spans="1:5" ht="136" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
-        <v>33</v>
+        <v>23</v>
       </c>
       <c r="B14" s="1">
         <v>5</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="E14" s="3"/>
     </row>
     <row r="15" spans="1:5" ht="170" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="B15" s="1">
         <v>5</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>35</v>
+        <v>45</v>
       </c>
       <c r="E15" s="3"/>
     </row>
-    <row r="16" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" ht="85" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
-        <v>39</v>
+        <v>28</v>
       </c>
       <c r="B16" s="1">
         <v>5</v>
       </c>
       <c r="C16" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D16" s="1" t="s">
         <v>40</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="B17" s="1">
         <v>5</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>44</v>
+        <v>31</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -830,8 +824,8 @@
     <hyperlink ref="A5" r:id="rId9" xr:uid="{644B3F42-DD28-7E44-BFEA-451702DF50F2}"/>
     <hyperlink ref="A4" r:id="rId10" xr:uid="{9C7531CA-CC48-C246-9C5A-1F24886375AA}"/>
     <hyperlink ref="A3" r:id="rId11" xr:uid="{1C8B91C2-3B6B-044E-9168-24498F7CE141}"/>
-    <hyperlink ref="D3" r:id="rId12" xr:uid="{17CF8206-DC49-024F-B798-7C575B61F1B3}"/>
-    <hyperlink ref="D6" r:id="rId13" xr:uid="{815E8B3B-5331-9840-B7FE-8FFDF4FBF2C9}"/>
+    <hyperlink ref="A2" r:id="rId12" xr:uid="{A4B7B17A-AD65-D549-B57F-946EC5B5518E}"/>
+    <hyperlink ref="D2" r:id="rId13" xr:uid="{D8C14069-FF2F-3845-BB02-DD364A0DD733}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>